<commit_message>
[feat][OOAD][Class diagram, Use case]
</commit_message>
<xml_diff>
--- a/System-Design-Architecture/Documents.xlsx
+++ b/System-Design-Architecture/Documents.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="507">
   <si>
     <t xml:space="preserve">Kiến Trúc về Microservice</t>
   </si>
@@ -1917,8 +1917,46 @@
         <family val="0"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> - With a good use case complete, textual analysis is a quick and easy way to figure out the classes in your system.</t>
-    </r>
+      <t xml:space="preserve"> - With a good use case complete, textual analysis is a quick and easy way to figure out the classes in your system.
+ - Pay attention to the </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">nouns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> in your use case, even when they aren’t classes in your system. Think about how the classes you do have can support the behavior describes.
+ - The verbs in your use case are (usually) the methods of the objects in your system.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Bullet points</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Analysis helps you ensure that your software works in the real world context, and not just in a perfect environment.
+ - Use cases are meant to be understood by you,your managers, your customers, and other programmers.
+ - You should write your use cases in whatever format makes them most usable to you and the other people who are looking at them
+ - A good use case precisely(chính xác) lays out what a system does, but does not indicate how the system accomplishes that task
+ - Each use case should focus on only one customer goal. If you have multiple goals you will need to write multiple use cases.
+ - Class diagram give an easy way to show your system and its code constructs at a 10000-foot view. The attributes in a class diagram usually map to the member variables of your classes.
+ - The operations in a class diagram usually represent the methods of your classes.
+ - Class diagram leave lots of detail out, such as class constructors, some type information, and the purpose of operations on your classes.
+ - Textual analysis helps you translate a use case into code-level classes, attributes, and operations.
+ - The nouns of a use case are candidates for classes in your system, and the verbs are candidates for the methods on your system’s classes.</t>
   </si>
   <si>
     <t xml:space="preserve">HEAD FIRST DESIGN PATTERN</t>
@@ -2762,9 +2800,6 @@
     <t xml:space="preserve">Favor composition over inheritance:
  - The Observer Pattern uses composition to compose any number of Observers with their Subject.
  - These relationships are set up at runtime by composition.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bullet points</t>
   </si>
   <si>
     <t xml:space="preserve"> - The Observer Pattern defines a one-to-many relationship between objects.
@@ -12099,7 +12134,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -12186,6 +12221,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -12486,9 +12525,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>588600</xdr:colOff>
+      <xdr:colOff>588240</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2121480</xdr:rowOff>
+      <xdr:rowOff>2121120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12502,7 +12541,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10237320" y="8324640"/>
-          <a:ext cx="4801320" cy="2798640"/>
+          <a:ext cx="4800960" cy="2798280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12523,9 +12562,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>664920</xdr:colOff>
+      <xdr:colOff>664560</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1797480</xdr:rowOff>
+      <xdr:rowOff>1797120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12539,7 +12578,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10323000" y="11420280"/>
-          <a:ext cx="4791960" cy="2493720"/>
+          <a:ext cx="4791600" cy="2493360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12560,9 +12599,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>522000</xdr:colOff>
+      <xdr:colOff>521640</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>696240</xdr:rowOff>
+      <xdr:rowOff>695880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12576,7 +12615,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10170720" y="24355440"/>
-          <a:ext cx="4801320" cy="2903400"/>
+          <a:ext cx="4800960" cy="2903040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12602,9 +12641,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>292680</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>280080</xdr:rowOff>
+      <xdr:rowOff>279720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12618,7 +12657,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15397560" y="67237200"/>
-          <a:ext cx="2792160" cy="1208880"/>
+          <a:ext cx="2791800" cy="1208520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12639,9 +12678,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>46440</xdr:colOff>
+      <xdr:colOff>46080</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:rowOff>12240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12655,7 +12694,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18540720" y="67199040"/>
-          <a:ext cx="2574360" cy="1284480"/>
+          <a:ext cx="2574000" cy="1284120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12676,9 +12715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>209520</xdr:colOff>
+      <xdr:colOff>209160</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>336240</xdr:rowOff>
+      <xdr:rowOff>335880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12692,7 +12731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15445080" y="68999400"/>
-          <a:ext cx="4564440" cy="1331640"/>
+          <a:ext cx="4564080" cy="1331280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12713,9 +12752,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>292680</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>280080</xdr:rowOff>
+      <xdr:rowOff>279720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12729,7 +12768,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15397560" y="67237200"/>
-          <a:ext cx="2792160" cy="1208880"/>
+          <a:ext cx="2791800" cy="1208520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12750,9 +12789,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>46440</xdr:colOff>
+      <xdr:colOff>46080</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:rowOff>12240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12766,7 +12805,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18540720" y="67199040"/>
-          <a:ext cx="2574360" cy="1284480"/>
+          <a:ext cx="2574000" cy="1284120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12787,9 +12826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>209520</xdr:colOff>
+      <xdr:colOff>209160</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>336240</xdr:rowOff>
+      <xdr:rowOff>335880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12803,7 +12842,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15445080" y="68999400"/>
-          <a:ext cx="4564440" cy="1331640"/>
+          <a:ext cx="4564080" cy="1331280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12829,9 +12868,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>46800</xdr:colOff>
+      <xdr:colOff>46440</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>389880</xdr:rowOff>
+      <xdr:rowOff>389520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12845,7 +12884,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11856600" y="0"/>
-          <a:ext cx="8208000" cy="4199400"/>
+          <a:ext cx="8207640" cy="4199040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13275,18 +13314,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>432</v>
-      </c>
-      <c r="B2" s="38" t="s">
         <v>433</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -13313,79 +13352,79 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="21.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="63" width="47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="64" width="125"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="35" width="60"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="35" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="64" width="47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="65" width="125"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="36" width="60"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="36" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="121.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="65" t="s">
-        <v>434</v>
-      </c>
-      <c r="B1" s="66" t="s">
+      <c r="A1" s="66" t="s">
         <v>435</v>
       </c>
+      <c r="B1" s="67" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="138.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="65"/>
-      <c r="B2" s="66" t="s">
-        <v>436</v>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="172.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="63" t="s">
-        <v>437</v>
-      </c>
-      <c r="B3" s="66" t="s">
+      <c r="A3" s="64" t="s">
         <v>438</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="B3" s="67" t="s">
         <v>439</v>
       </c>
+      <c r="C3" s="68" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="63" t="s">
-        <v>440</v>
-      </c>
-      <c r="B4" s="66" t="s">
+      <c r="A4" s="64" t="s">
         <v>441</v>
+      </c>
+      <c r="B4" s="67" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="66.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>442</v>
-      </c>
-      <c r="B5" s="66"/>
+        <v>443</v>
+      </c>
+      <c r="B5" s="67"/>
     </row>
     <row r="6" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="63" t="s">
-        <v>443</v>
-      </c>
-      <c r="B6" s="66"/>
+      <c r="A6" s="64" t="s">
+        <v>444</v>
+      </c>
+      <c r="B6" s="67"/>
     </row>
     <row r="7" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="63" t="s">
-        <v>444</v>
-      </c>
-      <c r="B7" s="66"/>
+      <c r="A7" s="64" t="s">
+        <v>445</v>
+      </c>
+      <c r="B7" s="67"/>
     </row>
     <row r="8" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="63" t="s">
-        <v>445</v>
+      <c r="A8" s="64" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="63" t="s">
-        <v>446</v>
-      </c>
-      <c r="B9" s="66" t="s">
+      <c r="A9" s="64" t="s">
         <v>447</v>
       </c>
+      <c r="B9" s="67" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="63" t="s">
-        <v>448</v>
+      <c r="A10" s="64" t="s">
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -13418,304 +13457,304 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="57" width="38.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="57" width="110.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="58" width="38.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="58" width="110.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="68" t="s">
-        <v>449</v>
-      </c>
-      <c r="B1" s="41" t="s">
+      <c r="A1" s="69" t="s">
         <v>450</v>
       </c>
+      <c r="B1" s="42" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="68"/>
-      <c r="B2" s="39" t="s">
-        <v>451</v>
+      <c r="A2" s="69"/>
+      <c r="B2" s="40" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="68"/>
-      <c r="B3" s="39" t="s">
-        <v>452</v>
+      <c r="A3" s="69"/>
+      <c r="B3" s="40" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="68" t="s">
-        <v>453</v>
-      </c>
-      <c r="B4" s="39" t="s">
+      <c r="A4" s="69" t="s">
         <v>454</v>
       </c>
+      <c r="B4" s="40" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="68"/>
-      <c r="B5" s="39" t="s">
-        <v>455</v>
+      <c r="A5" s="69"/>
+      <c r="B5" s="40" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="68"/>
-      <c r="B6" s="39" t="s">
-        <v>456</v>
+      <c r="A6" s="69"/>
+      <c r="B6" s="40" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="68" t="s">
-        <v>457</v>
-      </c>
-      <c r="B7" s="39" t="s">
+      <c r="A7" s="69" t="s">
         <v>458</v>
       </c>
+      <c r="B7" s="40" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="68"/>
-      <c r="B8" s="39" t="s">
-        <v>459</v>
+      <c r="A8" s="69"/>
+      <c r="B8" s="40" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="68"/>
-      <c r="B9" s="39" t="s">
-        <v>460</v>
+      <c r="A9" s="69"/>
+      <c r="B9" s="40" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="68"/>
-      <c r="B10" s="39" t="s">
-        <v>461</v>
+      <c r="A10" s="69"/>
+      <c r="B10" s="40" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="68"/>
-      <c r="B11" s="39" t="s">
-        <v>462</v>
+      <c r="A11" s="69"/>
+      <c r="B11" s="40" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="68" t="s">
-        <v>463</v>
-      </c>
-      <c r="B12" s="39" t="s">
+      <c r="A12" s="69" t="s">
         <v>464</v>
       </c>
+      <c r="B12" s="40" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="68"/>
-      <c r="B13" s="39" t="s">
-        <v>465</v>
+      <c r="A13" s="69"/>
+      <c r="B13" s="40" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="68"/>
-      <c r="B14" s="39" t="s">
-        <v>466</v>
+      <c r="A14" s="69"/>
+      <c r="B14" s="40" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="68"/>
-      <c r="B15" s="39" t="s">
-        <v>467</v>
+      <c r="A15" s="69"/>
+      <c r="B15" s="40" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="68"/>
-      <c r="B16" s="39" t="s">
-        <v>468</v>
+      <c r="A16" s="69"/>
+      <c r="B16" s="40" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="68"/>
-      <c r="B17" s="39" t="s">
-        <v>469</v>
+      <c r="A17" s="69"/>
+      <c r="B17" s="40" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="68"/>
-      <c r="B18" s="39" t="s">
-        <v>470</v>
+      <c r="A18" s="69"/>
+      <c r="B18" s="40" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="68"/>
-      <c r="B19" s="39" t="s">
-        <v>471</v>
+      <c r="A19" s="69"/>
+      <c r="B19" s="40" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="68"/>
-      <c r="B20" s="69" t="s">
-        <v>472</v>
+      <c r="A20" s="69"/>
+      <c r="B20" s="70" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="70" t="s">
-        <v>473</v>
-      </c>
-      <c r="B21" s="39" t="s">
+      <c r="A21" s="71" t="s">
         <v>474</v>
       </c>
+      <c r="B21" s="40" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="70"/>
-      <c r="B22" s="39" t="s">
-        <v>475</v>
+      <c r="A22" s="71"/>
+      <c r="B22" s="40" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="70"/>
-      <c r="B23" s="39" t="s">
-        <v>476</v>
+      <c r="A23" s="71"/>
+      <c r="B23" s="40" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="70"/>
-      <c r="B24" s="39" t="s">
-        <v>477</v>
+      <c r="A24" s="71"/>
+      <c r="B24" s="40" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="70"/>
-      <c r="B25" s="39" t="s">
-        <v>478</v>
+      <c r="A25" s="71"/>
+      <c r="B25" s="40" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="70"/>
-      <c r="B26" s="39" t="s">
-        <v>479</v>
+      <c r="A26" s="71"/>
+      <c r="B26" s="40" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="70"/>
-      <c r="B27" s="39" t="s">
-        <v>480</v>
+      <c r="A27" s="71"/>
+      <c r="B27" s="40" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="70"/>
-      <c r="B28" s="69" t="s">
-        <v>481</v>
+      <c r="A28" s="71"/>
+      <c r="B28" s="70" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="40" t="s">
-        <v>482</v>
-      </c>
-      <c r="B29" s="39" t="s">
+      <c r="A29" s="41" t="s">
         <v>483</v>
       </c>
+      <c r="B29" s="40" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="40"/>
-      <c r="B30" s="39" t="s">
-        <v>484</v>
+      <c r="A30" s="41"/>
+      <c r="B30" s="40" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="40"/>
-      <c r="B31" s="39" t="s">
-        <v>485</v>
+      <c r="A31" s="41"/>
+      <c r="B31" s="40" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="40"/>
-      <c r="B32" s="39" t="s">
-        <v>486</v>
+      <c r="A32" s="41"/>
+      <c r="B32" s="40" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="40"/>
-      <c r="B33" s="39" t="s">
-        <v>487</v>
+      <c r="A33" s="41"/>
+      <c r="B33" s="40" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="70" t="s">
-        <v>488</v>
-      </c>
-      <c r="B34" s="41" t="s">
+      <c r="A34" s="71" t="s">
         <v>489</v>
       </c>
+      <c r="B34" s="42" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="70"/>
-      <c r="B35" s="41" t="s">
-        <v>490</v>
+      <c r="A35" s="71"/>
+      <c r="B35" s="42" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="70"/>
-      <c r="B36" s="41" t="s">
-        <v>491</v>
+      <c r="A36" s="71"/>
+      <c r="B36" s="42" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="70"/>
-      <c r="B37" s="41" t="s">
-        <v>492</v>
+      <c r="A37" s="71"/>
+      <c r="B37" s="42" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="68" t="s">
-        <v>493</v>
-      </c>
-      <c r="B38" s="41" t="s">
+      <c r="A38" s="69" t="s">
         <v>494</v>
       </c>
+      <c r="B38" s="42" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="68"/>
-      <c r="B39" s="41" t="s">
-        <v>495</v>
+      <c r="A39" s="69"/>
+      <c r="B39" s="42" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="68"/>
-      <c r="B40" s="41" t="s">
-        <v>496</v>
+      <c r="A40" s="69"/>
+      <c r="B40" s="42" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="68"/>
-      <c r="B41" s="41" t="s">
-        <v>497</v>
+      <c r="A41" s="69"/>
+      <c r="B41" s="42" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="68"/>
-      <c r="B42" s="41" t="s">
-        <v>498</v>
+      <c r="A42" s="69"/>
+      <c r="B42" s="42" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="68"/>
-      <c r="B43" s="41" t="s">
-        <v>499</v>
+      <c r="A43" s="69"/>
+      <c r="B43" s="42" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="71"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="72"/>
+      <c r="B44" s="42"/>
     </row>
     <row r="45" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="72" t="s">
-        <v>500</v>
-      </c>
-      <c r="B45" s="72"/>
+      <c r="A45" s="73" t="s">
+        <v>501</v>
+      </c>
+      <c r="B45" s="73"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="72"/>
-      <c r="B46" s="72"/>
+      <c r="A46" s="73"/>
+      <c r="B46" s="73"/>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="71" t="s">
-        <v>501</v>
-      </c>
-      <c r="B47" s="73" t="s">
+      <c r="A47" s="72" t="s">
         <v>502</v>
+      </c>
+      <c r="B47" s="74" t="s">
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -13895,25 +13934,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="57" width="149.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="58" width="149.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="41" t="s">
-        <v>503</v>
+      <c r="B1" s="42" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="41" t="s">
-        <v>504</v>
+      <c r="A3" s="42" t="s">
+        <v>505</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="74"/>
+      <c r="B4" s="75"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -13933,8 +13972,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="121" zoomScaleNormal="121" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="121" zoomScaleNormal="121" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="21.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14166,7 +14205,7 @@
       </c>
       <c r="D22" s="16"/>
     </row>
-    <row r="23" customFormat="false" ht="69.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="92.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="11"/>
       <c r="B23" s="8" t="s">
         <v>86</v>
@@ -14176,12 +14215,19 @@
       </c>
       <c r="D23" s="16"/>
     </row>
-    <row r="24" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="136.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="11"/>
+      <c r="B24" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="22"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
     <mergeCell ref="A1:A6"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:B4"/>
@@ -14205,6 +14251,7 @@
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -14229,350 +14276,350 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="30.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="29.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="27.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="11.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="25" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="25" width="116.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="29.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="27.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="11.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="26" width="116.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="A1" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="26"/>
-      <c r="B2" s="28" t="s">
-        <v>90</v>
+      <c r="A2" s="27"/>
+      <c r="B2" s="29" t="s">
+        <v>92</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26"/>
-      <c r="B3" s="28" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="29" t="s">
         <v>64</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27" t="s">
-        <v>93</v>
+      <c r="A4" s="27"/>
+      <c r="B4" s="28" t="s">
+        <v>95</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" customFormat="false" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="31" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="C7" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="32"/>
     </row>
     <row r="8" customFormat="false" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="E8" s="31"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="32"/>
     </row>
     <row r="9" customFormat="false" ht="69" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="31"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="32"/>
     </row>
     <row r="10" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>102</v>
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>104</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="30"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="31"/>
       <c r="D11" s="15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="26"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
     </row>
     <row r="13" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="13" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="15" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="13" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="136.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27" t="s">
-        <v>111</v>
+      <c r="A15" s="27"/>
+      <c r="B15" s="28" t="s">
+        <v>113</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
     </row>
     <row r="16" customFormat="false" ht="136.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="26"/>
-      <c r="B16" s="27"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="13" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E17" s="12"/>
     </row>
     <row r="18" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="26"/>
-      <c r="B18" s="27"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="13"/>
       <c r="D18" s="12" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E18" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="13"/>
       <c r="D19" s="12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E19" s="12"/>
     </row>
     <row r="20" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="26"/>
-      <c r="B20" s="27"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="13"/>
       <c r="D20" s="12" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E20" s="12"/>
     </row>
     <row r="21" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="26"/>
-      <c r="B21" s="27"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="14" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="26"/>
-      <c r="B22" s="27" t="s">
-        <v>121</v>
+      <c r="A22" s="27"/>
+      <c r="B22" s="28" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="28"/>
     </row>
     <row r="24" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="26"/>
-      <c r="B24" s="27"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="28"/>
     </row>
     <row r="25" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="26"/>
-      <c r="B25" s="27"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="28"/>
     </row>
     <row r="26" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="26"/>
-      <c r="B26" s="27"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="28"/>
     </row>
     <row r="27" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="26"/>
-      <c r="B27" s="23" t="s">
-        <v>122</v>
+      <c r="A27" s="27"/>
+      <c r="B27" s="24" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="26"/>
-      <c r="B28" s="23" t="s">
-        <v>123</v>
+      <c r="A28" s="27"/>
+      <c r="B28" s="24" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="26"/>
-      <c r="B29" s="23" t="s">
-        <v>124</v>
+      <c r="A29" s="27"/>
+      <c r="B29" s="24" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="26"/>
-      <c r="B30" s="23" t="s">
-        <v>125</v>
+      <c r="A30" s="27"/>
+      <c r="B30" s="24" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="26"/>
-      <c r="B31" s="23" t="s">
-        <v>126</v>
+      <c r="A31" s="27"/>
+      <c r="B31" s="24" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="26"/>
-      <c r="B32" s="23" t="s">
-        <v>127</v>
+      <c r="A32" s="27"/>
+      <c r="B32" s="24" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="26"/>
-      <c r="B33" s="23" t="s">
-        <v>128</v>
+      <c r="A33" s="27"/>
+      <c r="B33" s="24" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="26"/>
-      <c r="B34" s="23" t="s">
-        <v>129</v>
+      <c r="A34" s="27"/>
+      <c r="B34" s="24" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="26"/>
-      <c r="B35" s="23" t="s">
-        <v>130</v>
+      <c r="A35" s="27"/>
+      <c r="B35" s="24" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="26"/>
-      <c r="B36" s="23" t="s">
-        <v>131</v>
+      <c r="A36" s="27"/>
+      <c r="B36" s="24" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="26"/>
-      <c r="B37" s="23" t="s">
-        <v>132</v>
+      <c r="A37" s="27"/>
+      <c r="B37" s="24" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="26" t="s">
-        <v>133</v>
+      <c r="A38" s="27" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="26"/>
+      <c r="A39" s="27"/>
     </row>
     <row r="40" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="26"/>
+      <c r="A40" s="27"/>
     </row>
     <row r="41" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="26"/>
+      <c r="A41" s="27"/>
     </row>
     <row r="42" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="26"/>
+      <c r="A42" s="27"/>
     </row>
     <row r="43" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="22" t="s">
-        <v>134</v>
+      <c r="A43" s="23" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="33" t="s">
-        <v>135</v>
+      <c r="A44" s="34" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="33"/>
+      <c r="A45" s="34"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="33"/>
+      <c r="A46" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="29">
@@ -14629,1193 +14676,1193 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="24" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="20.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="20.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="14.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="35" width="167.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="35" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="36" width="167.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="36" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="B1" s="37" t="s">
+      <c r="A1" s="37" t="s">
         <v>137</v>
       </c>
+      <c r="B1" s="38" t="s">
+        <v>138</v>
+      </c>
       <c r="C1" s="14" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="377.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="36"/>
-      <c r="B2" s="37"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="95.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37" t="s">
-        <v>141</v>
+      <c r="A3" s="37"/>
+      <c r="B3" s="38" t="s">
+        <v>142</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="14" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="36"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="14" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="36"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="36"/>
-      <c r="B8" s="37"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="36"/>
-      <c r="B9" s="37"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="36"/>
-      <c r="B10" s="37"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="36"/>
-      <c r="B11" s="37"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36"/>
-      <c r="B12" s="37"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="107.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="36"/>
-      <c r="B13" s="37" t="s">
-        <v>159</v>
+      <c r="A13" s="37"/>
+      <c r="B13" s="38" t="s">
+        <v>160</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="36"/>
-      <c r="B14" s="37"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="36"/>
-      <c r="B15" s="37"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="36"/>
-      <c r="B16" s="37"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="13"/>
       <c r="D16" s="15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="13"/>
       <c r="D17" s="15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="36"/>
-      <c r="B18" s="37"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="13"/>
       <c r="D18" s="15" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="36"/>
-      <c r="B19" s="37"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="13"/>
       <c r="D19" s="15" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="36"/>
-      <c r="B20" s="37"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="13"/>
       <c r="D20" s="15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="36"/>
-      <c r="B21" s="37"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="13"/>
       <c r="D21" s="15" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="95.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="36"/>
-      <c r="B22" s="37"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="38"/>
       <c r="C22" s="13" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="36"/>
-      <c r="B23" s="37"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="38"/>
       <c r="C23" s="13"/>
       <c r="D23" s="15" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="36"/>
-      <c r="B24" s="37"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="38"/>
       <c r="C24" s="13"/>
       <c r="D24" s="15" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="36"/>
-      <c r="B25" s="37"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="38"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="38" t="s">
-        <v>175</v>
+      <c r="D25" s="39" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="36"/>
-      <c r="B26" s="37"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="38"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="38" t="s">
-        <v>176</v>
+      <c r="D26" s="39" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="36"/>
-      <c r="B27" s="37"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="38" t="s">
-        <v>177</v>
+      <c r="D27" s="39" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="36"/>
-      <c r="B28" s="37"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="13"/>
-      <c r="D28" s="38" t="s">
-        <v>178</v>
+      <c r="D28" s="39" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="36"/>
-      <c r="B29" s="37"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="38"/>
       <c r="C29" s="13"/>
       <c r="D29" s="15" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="36"/>
-      <c r="B30" s="37"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="38"/>
       <c r="C30" s="13"/>
-      <c r="D30" s="38" t="s">
-        <v>180</v>
+      <c r="D30" s="39" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="36"/>
-      <c r="B31" s="37"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="38"/>
       <c r="C31" s="13"/>
-      <c r="D31" s="38" t="s">
-        <v>181</v>
+      <c r="D31" s="39" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="36"/>
-      <c r="B32" s="37"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="13"/>
-      <c r="D32" s="38" t="s">
-        <v>182</v>
+      <c r="D32" s="39" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="36"/>
-      <c r="B33" s="37"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="38"/>
       <c r="C33" s="13"/>
       <c r="D33" s="15" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="36"/>
-      <c r="B34" s="37"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="38"/>
       <c r="C34" s="13"/>
-      <c r="D34" s="39" t="s">
-        <v>184</v>
+      <c r="D34" s="40" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="391" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="36"/>
-      <c r="B35" s="37"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="38"/>
       <c r="C35" s="13"/>
-      <c r="D35" s="38" t="s">
-        <v>185</v>
+      <c r="D35" s="39" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="377.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="36"/>
-      <c r="B36" s="37"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="38"/>
       <c r="C36" s="13"/>
-      <c r="D36" s="38" t="s">
-        <v>186</v>
+      <c r="D36" s="39" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="36"/>
-      <c r="B37" s="37"/>
+      <c r="A37" s="37"/>
+      <c r="B37" s="38"/>
       <c r="C37" s="13"/>
-      <c r="D37" s="38" t="s">
-        <v>187</v>
+      <c r="D37" s="39" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="36"/>
-      <c r="B38" s="37"/>
+      <c r="A38" s="37"/>
+      <c r="B38" s="38"/>
       <c r="C38" s="13"/>
       <c r="D38" s="15" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="36"/>
-      <c r="B39" s="37"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="38"/>
       <c r="C39" s="13"/>
       <c r="D39" s="15" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="36"/>
-      <c r="B40" s="37"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="38"/>
       <c r="C40" s="13"/>
       <c r="D40" s="15" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="36"/>
-      <c r="B41" s="37"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="38"/>
       <c r="C41" s="14" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D41" s="15"/>
     </row>
     <row r="42" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="36"/>
-      <c r="B42" s="37"/>
+      <c r="A42" s="37"/>
+      <c r="B42" s="38"/>
       <c r="C42" s="14" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="135.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="36"/>
-      <c r="B43" s="37" t="s">
-        <v>194</v>
-      </c>
-      <c r="C43" s="37" t="s">
+      <c r="A43" s="37"/>
+      <c r="B43" s="38" t="s">
         <v>195</v>
       </c>
+      <c r="C43" s="38" t="s">
+        <v>196</v>
+      </c>
       <c r="D43" s="15" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="431.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="36"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
       <c r="D44" s="15" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="592.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="36"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
+      <c r="A45" s="37"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
       <c r="D45" s="15" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="36"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
       <c r="D46" s="15" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="36"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
       <c r="D47" s="15" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="36"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
       <c r="D48" s="15" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="36"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
+      <c r="A49" s="37"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
       <c r="D49" s="15" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="36"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
       <c r="D50" s="15" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="36"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="40" t="s">
-        <v>204</v>
+      <c r="A51" s="37"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="41" t="s">
+        <v>205</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="36"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="40"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="41"/>
       <c r="D52" s="15" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="36"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="40"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="15" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="36"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="40"/>
+      <c r="A54" s="37"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="41"/>
       <c r="D54" s="15" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="36"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="40"/>
+      <c r="A55" s="37"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="41"/>
       <c r="D55" s="15" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="36"/>
-      <c r="B56" s="37"/>
+      <c r="A56" s="37"/>
+      <c r="B56" s="38"/>
       <c r="C56" s="14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D56" s="15"/>
     </row>
     <row r="57" customFormat="false" ht="498.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="36"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="37" t="s">
-        <v>211</v>
-      </c>
-      <c r="D57" s="39" t="s">
+      <c r="A57" s="37"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38" t="s">
         <v>212</v>
       </c>
+      <c r="D57" s="40" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="36"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="37"/>
+      <c r="A58" s="37"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
       <c r="D58" s="15" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="36"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
       <c r="D59" s="15" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="36"/>
-      <c r="B60" s="37"/>
-      <c r="C60" s="37"/>
+      <c r="A60" s="37"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="38"/>
       <c r="D60" s="15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="36"/>
-      <c r="B61" s="37"/>
+      <c r="A61" s="37"/>
+      <c r="B61" s="38"/>
       <c r="C61" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="36"/>
-      <c r="B62" s="37"/>
+      <c r="A62" s="37"/>
+      <c r="B62" s="38"/>
       <c r="C62" s="13"/>
       <c r="D62" s="15" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="36"/>
-      <c r="B63" s="37"/>
+      <c r="A63" s="37"/>
+      <c r="B63" s="38"/>
       <c r="C63" s="13"/>
       <c r="D63" s="15" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="36"/>
-      <c r="B64" s="37"/>
+      <c r="A64" s="37"/>
+      <c r="B64" s="38"/>
       <c r="C64" s="13"/>
       <c r="D64" s="15" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="36"/>
-      <c r="B65" s="37"/>
+      <c r="A65" s="37"/>
+      <c r="B65" s="38"/>
       <c r="C65" s="13"/>
       <c r="D65" s="15" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="36"/>
-      <c r="B66" s="37"/>
+      <c r="A66" s="37"/>
+      <c r="B66" s="38"/>
       <c r="C66" s="13"/>
       <c r="D66" s="15" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="36"/>
-      <c r="B67" s="37"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="38"/>
       <c r="C67" s="13" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="36"/>
-      <c r="B68" s="37"/>
+      <c r="A68" s="37"/>
+      <c r="B68" s="38"/>
       <c r="C68" s="13"/>
       <c r="D68" s="15" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="36"/>
-      <c r="B69" s="37"/>
+      <c r="A69" s="37"/>
+      <c r="B69" s="38"/>
       <c r="C69" s="13"/>
       <c r="D69" s="15" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="36"/>
-      <c r="B70" s="37"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="38"/>
       <c r="C70" s="13"/>
       <c r="D70" s="15" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="36"/>
-      <c r="B71" s="37"/>
+      <c r="A71" s="37"/>
+      <c r="B71" s="38"/>
       <c r="C71" s="13"/>
       <c r="D71" s="15" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="36"/>
-      <c r="B72" s="37"/>
+      <c r="A72" s="37"/>
+      <c r="B72" s="38"/>
       <c r="C72" s="13"/>
       <c r="D72" s="15" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="36"/>
-      <c r="B73" s="37"/>
+      <c r="A73" s="37"/>
+      <c r="B73" s="38"/>
       <c r="C73" s="13"/>
       <c r="D73" s="15" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="36"/>
-      <c r="B74" s="37"/>
+      <c r="A74" s="37"/>
+      <c r="B74" s="38"/>
       <c r="C74" s="13"/>
       <c r="D74" s="15" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="36"/>
-      <c r="B75" s="37"/>
+      <c r="A75" s="37"/>
+      <c r="B75" s="38"/>
       <c r="C75" s="13"/>
       <c r="D75" s="15" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="36"/>
-      <c r="B76" s="37"/>
+      <c r="A76" s="37"/>
+      <c r="B76" s="38"/>
       <c r="C76" s="13"/>
       <c r="D76" s="15" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="36"/>
-      <c r="B77" s="37"/>
+      <c r="A77" s="37"/>
+      <c r="B77" s="38"/>
       <c r="C77" s="13"/>
-      <c r="D77" s="38" t="s">
-        <v>233</v>
+      <c r="D77" s="39" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="36"/>
-      <c r="B78" s="37"/>
+      <c r="A78" s="37"/>
+      <c r="B78" s="38"/>
       <c r="D78" s="15" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="36"/>
-      <c r="B79" s="37"/>
+      <c r="A79" s="37"/>
+      <c r="B79" s="38"/>
       <c r="C79" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D79" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="36"/>
-      <c r="B80" s="37"/>
-      <c r="C80" s="40" t="s">
-        <v>237</v>
+      <c r="A80" s="37"/>
+      <c r="B80" s="38"/>
+      <c r="C80" s="41" t="s">
+        <v>238</v>
       </c>
       <c r="D80" s="15" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="36"/>
-      <c r="B81" s="37"/>
-      <c r="C81" s="40"/>
-      <c r="D81" s="39" t="s">
-        <v>239</v>
+      <c r="A81" s="37"/>
+      <c r="B81" s="38"/>
+      <c r="C81" s="41"/>
+      <c r="D81" s="40" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="36"/>
-      <c r="B82" s="37"/>
-      <c r="C82" s="40"/>
-      <c r="D82" s="41" t="s">
-        <v>240</v>
+      <c r="A82" s="37"/>
+      <c r="B82" s="38"/>
+      <c r="C82" s="41"/>
+      <c r="D82" s="42" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="36"/>
-      <c r="B83" s="37"/>
-      <c r="C83" s="40"/>
-      <c r="D83" s="41" t="s">
-        <v>241</v>
+      <c r="A83" s="37"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="41"/>
+      <c r="D83" s="42" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="36"/>
-      <c r="B84" s="37"/>
-      <c r="C84" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="D84" s="41" t="s">
+      <c r="A84" s="37"/>
+      <c r="B84" s="38"/>
+      <c r="C84" s="38" t="s">
         <v>243</v>
       </c>
+      <c r="D84" s="42" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="36"/>
-      <c r="B85" s="37" t="s">
-        <v>244</v>
-      </c>
-      <c r="C85" s="37"/>
-      <c r="D85" s="41"/>
+      <c r="A85" s="37"/>
+      <c r="B85" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="C85" s="38"/>
+      <c r="D85" s="42"/>
     </row>
     <row r="86" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="36"/>
-      <c r="B86" s="37" t="s">
-        <v>245</v>
-      </c>
-      <c r="C86" s="37"/>
-      <c r="D86" s="41"/>
+      <c r="A86" s="37"/>
+      <c r="B86" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="C86" s="38"/>
+      <c r="D86" s="42"/>
     </row>
     <row r="87" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="36"/>
-      <c r="B87" s="37" t="s">
-        <v>246</v>
-      </c>
-      <c r="C87" s="37"/>
-      <c r="D87" s="41"/>
+      <c r="A87" s="37"/>
+      <c r="B87" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="C87" s="38"/>
+      <c r="D87" s="42"/>
     </row>
     <row r="88" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="36"/>
-      <c r="B88" s="37" t="s">
-        <v>247</v>
-      </c>
-      <c r="C88" s="37"/>
-      <c r="D88" s="41"/>
+      <c r="A88" s="37"/>
+      <c r="B88" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="C88" s="38"/>
+      <c r="D88" s="42"/>
     </row>
     <row r="89" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="36"/>
-      <c r="B89" s="37" t="s">
-        <v>248</v>
-      </c>
-      <c r="C89" s="37"/>
-      <c r="D89" s="41"/>
+      <c r="A89" s="37"/>
+      <c r="B89" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="C89" s="38"/>
+      <c r="D89" s="42"/>
     </row>
     <row r="90" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="36"/>
-      <c r="B90" s="37" t="s">
-        <v>249</v>
-      </c>
-      <c r="C90" s="37"/>
-      <c r="D90" s="41"/>
+      <c r="A90" s="37"/>
+      <c r="B90" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="C90" s="38"/>
+      <c r="D90" s="42"/>
     </row>
     <row r="91" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="36"/>
-      <c r="B91" s="37" t="s">
-        <v>250</v>
-      </c>
-      <c r="C91" s="37"/>
-      <c r="D91" s="41"/>
+      <c r="A91" s="37"/>
+      <c r="B91" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="C91" s="38"/>
+      <c r="D91" s="42"/>
     </row>
     <row r="92" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="36"/>
-      <c r="B92" s="37" t="s">
-        <v>251</v>
-      </c>
-      <c r="C92" s="37"/>
-      <c r="D92" s="41"/>
+      <c r="A92" s="37"/>
+      <c r="B92" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="C92" s="38"/>
+      <c r="D92" s="42"/>
     </row>
     <row r="93" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="36"/>
-      <c r="B93" s="42" t="s">
-        <v>252</v>
-      </c>
-      <c r="C93" s="37"/>
-      <c r="D93" s="41"/>
+      <c r="A93" s="37"/>
+      <c r="B93" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="C93" s="38"/>
+      <c r="D93" s="42"/>
     </row>
     <row r="94" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="36"/>
-      <c r="B94" s="37" t="s">
-        <v>253</v>
-      </c>
-      <c r="C94" s="37"/>
-      <c r="D94" s="41"/>
+      <c r="A94" s="37"/>
+      <c r="B94" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="C94" s="38"/>
+      <c r="D94" s="42"/>
     </row>
     <row r="95" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="36"/>
-      <c r="B95" s="42" t="s">
-        <v>254</v>
-      </c>
-      <c r="C95" s="37"/>
-      <c r="D95" s="41"/>
+      <c r="A95" s="37"/>
+      <c r="B95" s="43" t="s">
+        <v>255</v>
+      </c>
+      <c r="C95" s="38"/>
+      <c r="D95" s="42"/>
     </row>
     <row r="96" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="36"/>
-      <c r="B96" s="42" t="s">
-        <v>255</v>
-      </c>
-      <c r="C96" s="37"/>
-      <c r="D96" s="41"/>
+      <c r="A96" s="37"/>
+      <c r="B96" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="C96" s="38"/>
+      <c r="D96" s="42"/>
     </row>
     <row r="97" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="36"/>
-      <c r="B97" s="42" t="s">
-        <v>256</v>
-      </c>
-      <c r="C97" s="37"/>
-      <c r="D97" s="41"/>
+      <c r="A97" s="37"/>
+      <c r="B97" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="C97" s="38"/>
+      <c r="D97" s="42"/>
     </row>
     <row r="98" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="36"/>
-      <c r="B98" s="42" t="s">
-        <v>257</v>
-      </c>
-      <c r="C98" s="37"/>
-      <c r="D98" s="41"/>
+      <c r="A98" s="37"/>
+      <c r="B98" s="43" t="s">
+        <v>258</v>
+      </c>
+      <c r="C98" s="38"/>
+      <c r="D98" s="42"/>
     </row>
     <row r="99" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="36"/>
-      <c r="B99" s="42" t="s">
-        <v>258</v>
-      </c>
-      <c r="C99" s="37"/>
-      <c r="D99" s="41"/>
+      <c r="A99" s="37"/>
+      <c r="B99" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="C99" s="38"/>
+      <c r="D99" s="42"/>
     </row>
     <row r="100" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="36"/>
-      <c r="B100" s="37" t="s">
-        <v>259</v>
-      </c>
-      <c r="C100" s="37"/>
-      <c r="D100" s="41"/>
+      <c r="A100" s="37"/>
+      <c r="B100" s="38" t="s">
+        <v>260</v>
+      </c>
+      <c r="C100" s="38"/>
+      <c r="D100" s="42"/>
     </row>
     <row r="101" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="36"/>
-      <c r="B101" s="37" t="s">
-        <v>260</v>
-      </c>
-      <c r="C101" s="37"/>
-      <c r="D101" s="41"/>
+      <c r="A101" s="37"/>
+      <c r="B101" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="C101" s="38"/>
+      <c r="D101" s="42"/>
     </row>
     <row r="102" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="36"/>
-      <c r="B102" s="42" t="s">
-        <v>261</v>
-      </c>
-      <c r="C102" s="37"/>
-      <c r="D102" s="41"/>
+      <c r="A102" s="37"/>
+      <c r="B102" s="43" t="s">
+        <v>262</v>
+      </c>
+      <c r="C102" s="38"/>
+      <c r="D102" s="42"/>
     </row>
     <row r="103" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="36"/>
-      <c r="B103" s="37" t="s">
-        <v>262</v>
-      </c>
-      <c r="C103" s="37"/>
-      <c r="D103" s="41"/>
+      <c r="A103" s="37"/>
+      <c r="B103" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="C103" s="38"/>
+      <c r="D103" s="42"/>
     </row>
     <row r="104" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="36"/>
-      <c r="B104" s="37" t="s">
-        <v>263</v>
-      </c>
-      <c r="C104" s="37"/>
-      <c r="D104" s="41"/>
+      <c r="A104" s="37"/>
+      <c r="B104" s="38" t="s">
+        <v>264</v>
+      </c>
+      <c r="C104" s="38"/>
+      <c r="D104" s="42"/>
     </row>
     <row r="105" customFormat="false" ht="162.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="36"/>
-      <c r="B105" s="43" t="s">
-        <v>264</v>
+      <c r="A105" s="37"/>
+      <c r="B105" s="44" t="s">
+        <v>265</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D105" s="15" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="36"/>
-      <c r="B106" s="43"/>
+      <c r="A106" s="37"/>
+      <c r="B106" s="44"/>
       <c r="C106" s="14" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D106" s="15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="323.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="36"/>
-      <c r="B107" s="43"/>
+      <c r="A107" s="37"/>
+      <c r="B107" s="44"/>
       <c r="C107" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="D107" s="41" t="s">
         <v>270</v>
       </c>
+      <c r="D107" s="42" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="36"/>
-      <c r="B108" s="43"/>
+      <c r="A108" s="37"/>
+      <c r="B108" s="44"/>
       <c r="C108" s="13"/>
-      <c r="D108" s="39" t="s">
-        <v>271</v>
+      <c r="D108" s="40" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="36"/>
-      <c r="B109" s="43"/>
+      <c r="A109" s="37"/>
+      <c r="B109" s="44"/>
       <c r="C109" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="D109" s="41" t="s">
         <v>273</v>
       </c>
+      <c r="D109" s="42" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="256.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="36"/>
-      <c r="B110" s="43"/>
+      <c r="A110" s="37"/>
+      <c r="B110" s="44"/>
       <c r="C110" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="D110" s="39" t="s">
         <v>275</v>
       </c>
+      <c r="D110" s="40" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="404.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="36"/>
-      <c r="B111" s="43"/>
+      <c r="A111" s="37"/>
+      <c r="B111" s="44"/>
       <c r="C111" s="13"/>
-      <c r="D111" s="41" t="s">
-        <v>276</v>
+      <c r="D111" s="42" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="404.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="36"/>
-      <c r="B112" s="43"/>
+      <c r="A112" s="37"/>
+      <c r="B112" s="44"/>
       <c r="C112" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="D112" s="41" t="s">
         <v>278</v>
       </c>
+      <c r="D112" s="42" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="36"/>
-      <c r="B113" s="44"/>
+      <c r="A113" s="37"/>
+      <c r="B113" s="45"/>
       <c r="C113" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="D113" s="38" t="s">
         <v>280</v>
       </c>
+      <c r="D113" s="39" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="36"/>
-      <c r="B114" s="44"/>
+      <c r="A114" s="37"/>
+      <c r="B114" s="45"/>
       <c r="C114" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="D114" s="38" t="s">
         <v>282</v>
       </c>
+      <c r="D114" s="39" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="95.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="36"/>
-      <c r="B115" s="44"/>
+      <c r="A115" s="37"/>
+      <c r="B115" s="45"/>
       <c r="C115" s="13" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D115" s="15" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="36"/>
-      <c r="B116" s="44"/>
+      <c r="A116" s="37"/>
+      <c r="B116" s="45"/>
       <c r="C116" s="13"/>
       <c r="D116" s="15" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="36"/>
-      <c r="B117" s="44"/>
+      <c r="A117" s="37"/>
+      <c r="B117" s="45"/>
       <c r="C117" s="14" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D117" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="274.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="36"/>
+      <c r="A118" s="37"/>
       <c r="B118" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="C118" s="29" t="s">
         <v>289</v>
       </c>
-      <c r="D118" s="29"/>
+      <c r="C118" s="30" t="s">
+        <v>290</v>
+      </c>
+      <c r="D118" s="30"/>
     </row>
     <row r="119" customFormat="false" ht="243.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="36"/>
+      <c r="A119" s="37"/>
       <c r="B119" s="13"/>
-      <c r="C119" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="D119" s="29"/>
+      <c r="C119" s="30" t="s">
+        <v>291</v>
+      </c>
+      <c r="D119" s="30"/>
     </row>
     <row r="120" customFormat="false" ht="391.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="36"/>
+      <c r="A120" s="37"/>
       <c r="B120" s="13" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D120" s="12"/>
     </row>
     <row r="121" customFormat="false" ht="231" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="36"/>
+      <c r="A121" s="37"/>
       <c r="B121" s="13"/>
-      <c r="C121" s="29" t="s">
-        <v>293</v>
-      </c>
-      <c r="D121" s="29"/>
+      <c r="C121" s="30" t="s">
+        <v>294</v>
+      </c>
+      <c r="D121" s="30"/>
     </row>
     <row r="122" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="45" t="s">
-        <v>294</v>
+      <c r="A122" s="46" t="s">
+        <v>295</v>
       </c>
       <c r="B122" s="14" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C122" s="12" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D122" s="12"/>
     </row>
     <row r="123" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="45"/>
+      <c r="A123" s="46"/>
       <c r="B123" s="13" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D123" s="15" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="45"/>
+      <c r="A124" s="46"/>
       <c r="B124" s="13"/>
       <c r="C124" s="14" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D124" s="15" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="45"/>
+      <c r="A125" s="46"/>
       <c r="B125" s="13"/>
       <c r="C125" s="14" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D125" s="15" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="45"/>
+      <c r="A126" s="46"/>
       <c r="B126" s="13"/>
       <c r="C126" s="14" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D126" s="15" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="55.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="45"/>
+      <c r="A127" s="46"/>
       <c r="B127" s="13" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D127" s="15" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="45"/>
+      <c r="A128" s="46"/>
       <c r="B128" s="13"/>
       <c r="C128" s="14" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D128" s="15" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="45"/>
+      <c r="A129" s="46"/>
       <c r="B129" s="13"/>
       <c r="C129" s="15" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D129" s="15"/>
     </row>
     <row r="130" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="45"/>
+      <c r="A130" s="46"/>
       <c r="B130" s="13"/>
       <c r="C130" s="15" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D130" s="15"/>
     </row>
     <row r="131" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="45"/>
+      <c r="A131" s="46"/>
       <c r="B131" s="13"/>
       <c r="C131" s="15" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D131" s="15"/>
     </row>
     <row r="132" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="45"/>
+      <c r="A132" s="46"/>
       <c r="B132" s="13"/>
       <c r="C132" s="15" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D132" s="15"/>
     </row>
     <row r="133" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="45"/>
+      <c r="A133" s="46"/>
       <c r="B133" s="13" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D133" s="15"/>
     </row>
     <row r="134" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="45"/>
+      <c r="A134" s="46"/>
       <c r="B134" s="13"/>
       <c r="C134" s="15" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D134" s="15"/>
     </row>
     <row r="135" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="45"/>
+      <c r="A135" s="46"/>
       <c r="B135" s="13"/>
       <c r="C135" s="15" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D135" s="15"/>
     </row>
     <row r="136" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="45"/>
+      <c r="A136" s="46"/>
       <c r="B136" s="14" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C136" s="15"/>
       <c r="D136" s="15"/>
@@ -15908,205 +15955,205 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="24" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="55.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="47" width="54.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="48" width="101.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="55.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="48" width="54.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="49" width="101.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="49" t="s">
-        <v>320</v>
+      <c r="A1" s="50" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="49"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="52"/>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="49"/>
-      <c r="B4" s="50"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
+      <c r="A5" s="50"/>
+      <c r="B5" s="51"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="49"/>
-      <c r="B6" s="50"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="51"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="49"/>
-      <c r="B7" s="50"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="51"/>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="49"/>
-      <c r="B8" s="50"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="51"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="49"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="51"/>
     </row>
     <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="49"/>
-      <c r="B10" s="50"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="51"/>
     </row>
     <row r="11" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="49"/>
-      <c r="B11" s="50"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="51"/>
     </row>
     <row r="12" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="49"/>
-      <c r="B12" s="50"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="51"/>
     </row>
     <row r="13" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="49"/>
-      <c r="B13" s="50"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="51"/>
     </row>
     <row r="14" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="49"/>
-      <c r="B14" s="50"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="51"/>
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="49"/>
-      <c r="B15" s="50"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="51"/>
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="49"/>
-      <c r="B16" s="50"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="51"/>
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="49"/>
-      <c r="B17" s="50"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="51"/>
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="49"/>
-      <c r="B18" s="50"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="51"/>
     </row>
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="49"/>
-      <c r="B19" s="50"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="51"/>
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="49"/>
-      <c r="B20" s="50"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="51"/>
     </row>
     <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="49"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="51"/>
     </row>
     <row r="22" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="49"/>
-      <c r="B22" s="52"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="53"/>
     </row>
     <row r="23" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="49"/>
-      <c r="B23" s="52"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="53"/>
     </row>
     <row r="24" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="49"/>
-      <c r="B24" s="53"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="54"/>
     </row>
     <row r="26" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="49" t="s">
-        <v>321</v>
-      </c>
-      <c r="B26" s="47" t="s">
+      <c r="A26" s="50" t="s">
         <v>322</v>
       </c>
+      <c r="B26" s="48" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="49"/>
-      <c r="B27" s="47" t="s">
-        <v>323</v>
+      <c r="A27" s="50"/>
+      <c r="B27" s="48" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="49"/>
-      <c r="B28" s="47" t="s">
-        <v>324</v>
+      <c r="A28" s="50"/>
+      <c r="B28" s="48" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="54"/>
+      <c r="A29" s="55"/>
     </row>
     <row r="30" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="49" t="s">
-        <v>325</v>
-      </c>
-      <c r="B30" s="55" t="s">
+      <c r="A30" s="50" t="s">
         <v>326</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="B30" s="56" t="s">
         <v>327</v>
       </c>
+      <c r="C30" s="49" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="49"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="48" t="s">
-        <v>328</v>
+      <c r="A31" s="50"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="49" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="49"/>
-      <c r="B32" s="55"/>
-      <c r="C32" s="48" t="s">
-        <v>329</v>
+      <c r="A32" s="50"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="49" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="49"/>
-      <c r="B33" s="55"/>
-      <c r="C33" s="48" t="s">
-        <v>330</v>
+      <c r="A33" s="50"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="49" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="49" t="s">
-        <v>331</v>
-      </c>
-      <c r="B35" s="47" t="s">
+      <c r="A35" s="50" t="s">
         <v>332</v>
       </c>
-      <c r="C35" s="56" t="s">
+      <c r="B35" s="48" t="s">
         <v>333</v>
       </c>
+      <c r="C35" s="57" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="49"/>
-      <c r="B36" s="47" t="s">
-        <v>334</v>
-      </c>
-      <c r="C36" s="56" t="s">
+      <c r="A36" s="50"/>
+      <c r="B36" s="48" t="s">
         <v>335</v>
       </c>
+      <c r="C36" s="57" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="49"/>
-      <c r="B37" s="47" t="s">
-        <v>336</v>
-      </c>
-      <c r="C37" s="56" t="s">
+      <c r="A37" s="50"/>
+      <c r="B37" s="48" t="s">
         <v>337</v>
       </c>
+      <c r="C37" s="57" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="49"/>
-      <c r="B38" s="47" t="s">
-        <v>338</v>
-      </c>
-      <c r="C38" s="56" t="s">
+      <c r="A38" s="50"/>
+      <c r="B38" s="48" t="s">
         <v>339</v>
       </c>
+      <c r="C38" s="57" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="54" t="s">
-        <v>340</v>
+      <c r="A40" s="55" t="s">
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -16142,17 +16189,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="57" width="151.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="58" width="151.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1" s="41" t="s">
-        <v>341</v>
+      <c r="D1" s="42" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="349.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D2" s="41" t="s">
-        <v>342</v>
+      <c r="D2" s="42" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -16179,12 +16226,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="57" width="140"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="58" width="140"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="41" t="s">
-        <v>343</v>
+      <c r="C1" s="42" t="s">
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -16216,67 +16263,67 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="58" t="s">
-        <v>344</v>
+      <c r="A1" s="59" t="s">
+        <v>345</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="C1" s="59" t="s">
         <v>346</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="200.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -16284,240 +16331,240 @@
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="310.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="60"/>
+      <c r="B23" s="61"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="61" t="s">
-        <v>395</v>
+      <c r="A54" s="62" t="s">
+        <v>396</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="61"/>
+      <c r="A55" s="62"/>
       <c r="B55" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="61"/>
+      <c r="A56" s="62"/>
       <c r="B56" s="4" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="13" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="13"/>
-      <c r="B59" s="62" t="s">
-        <v>401</v>
+      <c r="B59" s="63" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="13"/>
-      <c r="B60" s="62" t="s">
-        <v>402</v>
+      <c r="B60" s="63" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="13"/>
-      <c r="B61" s="62" t="s">
-        <v>403</v>
+      <c r="B61" s="63" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="13"/>
-      <c r="B62" s="62" t="s">
-        <v>404</v>
+      <c r="B62" s="63" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="13"/>
-      <c r="B63" s="62" t="s">
-        <v>405</v>
+      <c r="B63" s="63" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="13"/>
-      <c r="B64" s="62" t="s">
-        <v>406</v>
+      <c r="B64" s="63" t="s">
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -16557,100 +16604,100 @@
   <sheetData>
     <row r="1" customFormat="false" ht="297" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13"/>
       <c r="B5" s="15" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="149.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="37" t="s">
-        <v>426</v>
+      <c r="A11" s="38" t="s">
+        <v>427</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="37"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="15" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="37"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="15" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>